<commit_message>
msz - second smoke test is running - new naming
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgTruckInsurance.xlsx
+++ b/Data/Dialogs/dlgTruckInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AF0323-1DE3-4227-8132-CD9D2AB47A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45864BF-999D-40E9-983B-DCE313D57498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="35280" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="39096" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
   <si>
     <t>Action</t>
   </si>
@@ -108,9 +108,6 @@
     <t>VIA_Pixel9Pro_API35</t>
   </si>
   <si>
-    <t>103_TruckInsuranceAutomobile_001_SmokeTest_FillPageVehicleData</t>
-  </si>
-  <si>
     <t>//*[@id="insurance-form"]/div/section[1]</t>
   </si>
   <si>
@@ -124,6 +121,45 @@
   </si>
   <si>
     <t>//*[@id="insurance-form"]/div/section[5]</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_001_SmokeTest_FillPageVehicleData</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_001_SmokeTest_FillPageInsurantData</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_001_SmokeTest_FillPageProductData</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_001_SmokeTest_FillPageSendQuote</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_001_SmokeTest_FillPage</t>
+  </si>
+  <si>
+    <t>Button Next from Page VehicleData</t>
+  </si>
+  <si>
+    <t>Button Next</t>
+  </si>
+  <si>
+    <t>Choose Silver</t>
+  </si>
+  <si>
+    <t>Choose Gold</t>
+  </si>
+  <si>
+    <t>Choose Platinum</t>
+  </si>
+  <si>
+    <t>Choose Ultimate</t>
+  </si>
+  <si>
+    <t>Send Quote - Button Main Page</t>
+  </si>
+  <si>
+    <t>Button Main Page</t>
   </si>
 </sst>
 </file>
@@ -206,15 +242,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2369905</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>6477</xdr:rowOff>
+      <xdr:colOff>129625</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>44577</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -237,7 +273,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4213860"/>
+          <a:off x="7620" y="4800600"/>
           <a:ext cx="14561905" cy="9142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -547,17 +583,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="A19" sqref="A19:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -568,19 +607,19 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -781,7 +820,142 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
msz - more testcases, 2 new selectDropdown keywords, Videorecording
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgTruckInsurance.xlsx
+++ b/Data/Dialogs/dlgTruckInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACF3B57-96C3-4BA1-B08B-3BA9CB458C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C23B79B-96CA-41ED-A415-475930849818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1992" yWindow="372" windowWidth="36948" windowHeight="15672" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="420" yWindow="1752" windowWidth="39612" windowHeight="13668" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
   <si>
     <t>Action</t>
   </si>
@@ -127,6 +127,60 @@
   </si>
   <si>
     <t>103_TruckInsurance_002_VehicleData_002_ManufacturingDateInTheFuture</t>
+  </si>
+  <si>
+    <t>Insurant Data Page check for open mandatory fields</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_003_InsurantData_001_MandatoryFields_FillFirstName</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_003_InsurantData_001_MandatoryFields_CheckFilledFirstName</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_003_InsurantData_002_EnterValuesInWrongFormat</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_003_InsurantData_002_EnterValuesInWrongFormat Part 2</t>
+  </si>
+  <si>
+    <t>Insurant Data Page check for hints regarding mandatory fields</t>
+  </si>
+  <si>
+    <t>Insurant Data Page check error hint formatting</t>
+  </si>
+  <si>
+    <t>Insurant Data Page check error hint formatting Part 2</t>
+  </si>
+  <si>
+    <t>Check for open mandatory fields</t>
+  </si>
+  <si>
+    <t>Check for hints regarding mandatory fields</t>
+  </si>
+  <si>
+    <t>Enter values in wrong format</t>
+  </si>
+  <si>
+    <t>Check error hint formatting</t>
+  </si>
+  <si>
+    <t>Enter values in wrong format part 2</t>
+  </si>
+  <si>
+    <t>Check error hint formatting Part 2</t>
+  </si>
+  <si>
+    <t>MandatoryFields_FillFirstName</t>
+  </si>
+  <si>
+    <t>MandatoryFields_CheckFilledFirstName</t>
+  </si>
+  <si>
+    <t>103_TruckInsurance_003_InsurantData_003_ListContents</t>
+  </si>
+  <si>
+    <t>List content</t>
   </si>
 </sst>
 </file>
@@ -209,15 +263,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>891625</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>21717</xdr:rowOff>
+      <xdr:colOff>1348825</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>29337</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -240,7 +294,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60960" y="3131820"/>
+          <a:off x="106680" y="5516880"/>
           <a:ext cx="14561905" cy="9142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -550,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,10 +615,9 @@
     <col min="1" max="1" width="71.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -817,6 +870,132 @@
         <v>3</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>